<commit_message>
Changes to be committed: 	modified:   __pycache__/libCrud.cpython-311.pyc 	modified:   data.db 	modified:   error.xlsx 	modified:   libCrud.py 	modified:   scrapt-xls.py
</commit_message>
<xml_diff>
--- a/error.xlsx
+++ b/error.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A2:A5"/>
@@ -469,16 +469,30 @@
       <c r="A3" s="3" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>OIIIIIIIII</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>ola</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>OIIIIIIIII</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BWK17ABANA</t>
         </is>
       </c>
     </row>

</xml_diff>